<commit_message>
fix showing of all values add logic for grouping button Needs to be fixed
</commit_message>
<xml_diff>
--- a/food/food/spiders/foods.xlsx
+++ b/food/food/spiders/foods.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,7 +51,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,79 +431,79 @@
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="13" customWidth="1" min="14" max="14"/>
-    <col width="13" customWidth="1" min="15" max="15"/>
-    <col width="14" customWidth="1" min="16" max="16"/>
-    <col width="13" customWidth="1" min="17" max="17"/>
-    <col width="16" customWidth="1" min="18" max="18"/>
-    <col width="26" customWidth="1" min="19" max="19"/>
-    <col width="30" customWidth="1" min="20" max="20"/>
-    <col width="26" customWidth="1" min="21" max="21"/>
-    <col width="25" customWidth="1" min="22" max="22"/>
-    <col width="40" customWidth="1" min="23" max="23"/>
-    <col width="30" customWidth="1" min="24" max="24"/>
-    <col width="37" customWidth="1" min="25" max="25"/>
-    <col width="32" customWidth="1" min="26" max="26"/>
-    <col width="16" customWidth="1" min="27" max="27"/>
-    <col width="17" customWidth="1" min="28" max="28"/>
-    <col width="16" customWidth="1" min="29" max="29"/>
-    <col width="18" customWidth="1" min="30" max="30"/>
-    <col width="25" customWidth="1" min="31" max="31"/>
-    <col width="15" customWidth="1" min="32" max="32"/>
-    <col width="13" customWidth="1" min="33" max="33"/>
-    <col width="27" customWidth="1" min="34" max="34"/>
-    <col width="11" customWidth="1" min="35" max="35"/>
-    <col width="12" customWidth="1" min="36" max="36"/>
-    <col width="14" customWidth="1" min="37" max="37"/>
-    <col width="15" customWidth="1" min="38" max="38"/>
-    <col width="12" customWidth="1" min="39" max="39"/>
-    <col width="11" customWidth="1" min="40" max="40"/>
-    <col width="14" customWidth="1" min="41" max="41"/>
-    <col width="12" customWidth="1" min="42" max="42"/>
-    <col width="11" customWidth="1" min="43" max="43"/>
-    <col width="13" customWidth="1" min="44" max="44"/>
-    <col width="13" customWidth="1" min="45" max="45"/>
-    <col width="15" customWidth="1" min="46" max="46"/>
-    <col width="17" customWidth="1" min="47" max="47"/>
-    <col width="20" customWidth="1" min="48" max="48"/>
-    <col width="14" customWidth="1" min="49" max="49"/>
-    <col width="12" customWidth="1" min="50" max="50"/>
-    <col width="13" customWidth="1" min="51" max="51"/>
-    <col width="28" customWidth="1" min="52" max="52"/>
-    <col width="28" customWidth="1" min="53" max="53"/>
-    <col width="22" customWidth="1" min="54" max="54"/>
-    <col width="18" customWidth="1" min="55" max="55"/>
-    <col width="13" customWidth="1" min="56" max="56"/>
-    <col width="12" customWidth="1" min="57" max="57"/>
-    <col width="13" customWidth="1" min="58" max="58"/>
-    <col width="14" customWidth="1" min="59" max="59"/>
-    <col width="11" customWidth="1" min="60" max="60"/>
-    <col width="10" customWidth="1" min="61" max="61"/>
-    <col width="13" customWidth="1" min="62" max="62"/>
-    <col width="13" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
-    <col width="13" customWidth="1" min="65" max="65"/>
-    <col width="11" customWidth="1" min="66" max="66"/>
-    <col width="17" customWidth="1" min="67" max="67"/>
-    <col width="18" customWidth="1" min="68" max="68"/>
-    <col width="19" customWidth="1" min="69" max="69"/>
-    <col width="19" customWidth="1" min="70" max="70"/>
-    <col width="23" customWidth="1" min="71" max="71"/>
-    <col width="13" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
-    <col width="13" customWidth="1" min="74" max="74"/>
-    <col width="16" customWidth="1" min="75" max="75"/>
-    <col width="11" customWidth="1" min="76" max="76"/>
+    <col outlineLevel="1" width="20" customWidth="1" min="4" max="4"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="5" max="5"/>
+    <col outlineLevel="1" width="18" customWidth="1" min="6" max="6"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="7" max="7"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="8" max="8"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="9" max="9"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="10" max="10"/>
+    <col outlineLevel="1" width="15" customWidth="1" min="11" max="11"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="12" max="12"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="13" max="13"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="14" max="14"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="15" max="15"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="16" max="16"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="17" max="17"/>
+    <col outlineLevel="1" width="16" customWidth="1" min="18" max="18"/>
+    <col outlineLevel="1" width="26" customWidth="1" min="19" max="19"/>
+    <col outlineLevel="1" width="30" customWidth="1" min="20" max="20"/>
+    <col outlineLevel="1" width="26" customWidth="1" min="21" max="21"/>
+    <col outlineLevel="1" width="25" customWidth="1" min="22" max="22"/>
+    <col outlineLevel="1" width="40" customWidth="1" min="23" max="23"/>
+    <col outlineLevel="1" width="30" customWidth="1" min="24" max="24"/>
+    <col outlineLevel="1" width="37" customWidth="1" min="25" max="25"/>
+    <col outlineLevel="1" width="32" customWidth="1" min="26" max="26"/>
+    <col outlineLevel="1" width="16" customWidth="1" min="27" max="27"/>
+    <col outlineLevel="1" width="17" customWidth="1" min="28" max="28"/>
+    <col outlineLevel="1" width="16" customWidth="1" min="29" max="29"/>
+    <col outlineLevel="1" width="18" customWidth="1" min="30" max="30"/>
+    <col outlineLevel="1" width="25" customWidth="1" min="31" max="31"/>
+    <col outlineLevel="1" width="15" customWidth="1" min="32" max="32"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="33" max="33"/>
+    <col outlineLevel="1" width="27" customWidth="1" min="34" max="34"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="35" max="35"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="36" max="36"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="37" max="37"/>
+    <col outlineLevel="1" width="15" customWidth="1" min="38" max="38"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="39" max="39"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="40" max="40"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="41" max="41"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="42" max="42"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="43" max="43"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="44" max="44"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="45" max="45"/>
+    <col outlineLevel="1" width="15" customWidth="1" min="46" max="46"/>
+    <col outlineLevel="1" width="17" customWidth="1" min="47" max="47"/>
+    <col outlineLevel="1" width="20" customWidth="1" min="48" max="48"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="49" max="49"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="50" max="50"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="51" max="51"/>
+    <col outlineLevel="1" width="28" customWidth="1" min="52" max="52"/>
+    <col outlineLevel="1" width="28" customWidth="1" min="53" max="53"/>
+    <col outlineLevel="1" width="22" customWidth="1" min="54" max="54"/>
+    <col outlineLevel="1" width="18" customWidth="1" min="55" max="55"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="56" max="56"/>
+    <col outlineLevel="1" width="12" customWidth="1" min="57" max="57"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="58" max="58"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="59" max="59"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="60" max="60"/>
+    <col outlineLevel="1" width="10" customWidth="1" min="61" max="61"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="62" max="62"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="63" max="63"/>
+    <col outlineLevel="1" width="14" customWidth="1" min="64" max="64"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="65" max="65"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="66" max="66"/>
+    <col outlineLevel="1" width="17" customWidth="1" min="67" max="67"/>
+    <col outlineLevel="1" width="18" customWidth="1" min="68" max="68"/>
+    <col outlineLevel="1" width="19" customWidth="1" min="69" max="69"/>
+    <col outlineLevel="1" width="19" customWidth="1" min="70" max="70"/>
+    <col outlineLevel="1" width="23" customWidth="1" min="71" max="71"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="72" max="72"/>
+    <col outlineLevel="1" width="10" customWidth="1" min="73" max="73"/>
+    <col outlineLevel="1" width="13" customWidth="1" min="74" max="74"/>
+    <col outlineLevel="1" width="16" customWidth="1" min="75" max="75"/>
+    <col outlineLevel="1" width="11" customWidth="1" min="76" max="76"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -566,12 +569,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Калории</t>
+          <t>Калории (к)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Протеини (г)</t>
+          <t>Протеин (г)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -946,9 +949,15 @@
           <t>Зърнени култури</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>497</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56</v>
+      </c>
       <c r="G3" t="n">
         <v>26</v>
       </c>

</xml_diff>